<commit_message>
Added 2023 Rugby World Cup Round 2 forecasts
</commit_message>
<xml_diff>
--- a/seasons/AustralianRulesFootball/AustralianFootballLeague/2023/forecasts/ReportRoundSF_matrix.xlsx
+++ b/seasons/AustralianRulesFootball/AustralianFootballLeague/2023/forecasts/ReportRoundSF_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\SportPredictifier\main\SportPredictifier\seasons\AustralianRulesFootball\AustralianFootballLeague\2023\forecasts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21658DD9-2646-4354-B85D-BFFA635980BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A143A11-5686-4E7C-9763-A8462C541282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="41">
   <si>
     <t>Location</t>
   </si>
@@ -164,12 +164,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="#0.00"/>
     <numFmt numFmtId="165" formatCode="#0%"/>
     <numFmt numFmtId="166" formatCode="#0"/>
+    <numFmt numFmtId="167" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,6 +230,13 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -485,10 +493,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -517,27 +526,12 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -557,18 +551,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -599,9 +581,38 @@
     <xf numFmtId="166" fontId="6" fillId="10" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -906,7 +917,7 @@
   <dimension ref="B1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="E3" sqref="E3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -919,202 +930,202 @@
   <sheetData>
     <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="11"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="13"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="12"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B3" s="14"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="16" t="s">
+      <c r="B3" s="13"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="17"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="18"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="15"/>
     </row>
     <row r="4" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="14"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="19" t="s">
+      <c r="B4" s="13"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="20"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="18"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="15"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B5" s="14"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="30" t="s">
+      <c r="B5" s="13"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="31"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="18"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="15"/>
     </row>
     <row r="6" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="14"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="32" t="s">
+      <c r="B6" s="13"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="33"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="18"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="15"/>
     </row>
     <row r="7" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="14"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="18"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="15"/>
     </row>
     <row r="8" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="14"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="34" t="s">
+      <c r="B8" s="13"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="35" t="s">
+      <c r="F8" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="18"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="15"/>
     </row>
     <row r="9" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="14"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="43">
+      <c r="B9" s="13"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="34">
         <v>85.024054599999999</v>
       </c>
-      <c r="F9" s="26">
+      <c r="F9" s="21">
         <v>84.757022399999997</v>
       </c>
-      <c r="G9" s="24"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="18"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="15"/>
     </row>
     <row r="10" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="14"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="18"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="15"/>
     </row>
     <row r="11" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="14"/>
-      <c r="C11" s="34" t="s">
+      <c r="B11" s="13"/>
+      <c r="C11" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="40" t="s">
+      <c r="D11" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="36" t="s">
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="H11" s="37" t="s">
+      <c r="H11" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="I11" s="18"/>
+      <c r="I11" s="15"/>
     </row>
     <row r="12" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="14"/>
-      <c r="C12" s="43">
+      <c r="B12" s="13"/>
+      <c r="C12" s="34">
         <v>92.446858199999994</v>
       </c>
-      <c r="D12" s="26">
+      <c r="D12" s="21">
         <v>81.409833399999997</v>
       </c>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="43">
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="34">
         <v>84.721785800000006</v>
       </c>
-      <c r="H12" s="26">
+      <c r="H12" s="21">
         <v>81.651241999999996</v>
       </c>
-      <c r="I12" s="18"/>
+      <c r="I12" s="15"/>
     </row>
     <row r="13" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="14"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="18"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="15"/>
     </row>
     <row r="14" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="14"/>
-      <c r="C14" s="41" t="s">
+      <c r="B14" s="13"/>
+      <c r="C14" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="42" t="s">
+      <c r="D14" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="38" t="s">
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="H14" s="39" t="s">
+      <c r="H14" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="I14" s="18"/>
+      <c r="I14" s="15"/>
     </row>
     <row r="15" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="14"/>
-      <c r="C15" s="43">
+      <c r="B15" s="13"/>
+      <c r="C15" s="34">
         <v>91.527341399999997</v>
       </c>
-      <c r="D15" s="26">
+      <c r="D15" s="21">
         <v>89.005340200000006</v>
       </c>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="43">
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="34">
         <v>78.865211799999997</v>
       </c>
-      <c r="H15" s="26">
+      <c r="H15" s="21">
         <v>71.002081000000004</v>
       </c>
-      <c r="I15" s="18"/>
+      <c r="I15" s="15"/>
     </row>
     <row r="16" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="27"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="29"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1130,10 +1141,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B8E558B-6439-4C16-A744-54AC1151E8C4}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="B20" sqref="B20:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1389,7 +1400,63 @@
         <v>3.7635067376192863E-2</v>
       </c>
     </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="44">
+        <v>0.38707844323705609</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="44">
+        <v>0.33493556711111583</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="44">
+        <v>0.14399401895664732</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="44">
+        <v>5.6718649137835246E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="44">
+        <v>3.9638254181152723E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="44">
+        <v>3.7635067376192863E-2</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A20:B25">
+    <sortCondition descending="1" ref="B20:B25"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1534,66 +1601,66 @@
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="E2" s="10" t="s">
+      <c r="C2" s="43"/>
+      <c r="E2" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="10"/>
-      <c r="H2" s="10" t="s">
+      <c r="F2" s="43"/>
+      <c r="H2" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="10"/>
-      <c r="K2" s="10" t="s">
+      <c r="I2" s="43"/>
+      <c r="K2" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="L2" s="10"/>
-      <c r="N2" s="10" t="s">
+      <c r="L2" s="43"/>
+      <c r="N2" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="O2" s="10"/>
-      <c r="Q2" s="10" t="s">
+      <c r="O2" s="43"/>
+      <c r="Q2" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="10"/>
-      <c r="T2" s="10" t="s">
+      <c r="R2" s="43"/>
+      <c r="T2" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="U2" s="10"/>
-      <c r="W2" s="10" t="s">
+      <c r="U2" s="43"/>
+      <c r="W2" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="X2" s="10"/>
-      <c r="Z2" s="10" t="s">
+      <c r="X2" s="43"/>
+      <c r="Z2" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="AA2" s="10"/>
-      <c r="AC2" s="10" t="s">
+      <c r="AA2" s="43"/>
+      <c r="AC2" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="AD2" s="10"/>
-      <c r="AF2" s="10" t="s">
+      <c r="AD2" s="43"/>
+      <c r="AF2" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="AG2" s="10"/>
-      <c r="AI2" s="10" t="s">
+      <c r="AG2" s="43"/>
+      <c r="AI2" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="AJ2" s="10"/>
-      <c r="AL2" s="10" t="s">
+      <c r="AJ2" s="43"/>
+      <c r="AL2" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="AM2" s="10"/>
-      <c r="AO2" s="10" t="s">
+      <c r="AM2" s="43"/>
+      <c r="AO2" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="AP2" s="10"/>
-      <c r="AR2" s="10" t="s">
+      <c r="AP2" s="43"/>
+      <c r="AR2" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="AS2" s="10"/>
+      <c r="AS2" s="43"/>
     </row>
     <row r="3" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
@@ -3607,21 +3674,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="AC2:AD2"/>
     <mergeCell ref="AF2:AG2"/>
     <mergeCell ref="AI2:AJ2"/>
     <mergeCell ref="AL2:AM2"/>
     <mergeCell ref="AO2:AP2"/>
     <mergeCell ref="AR2:AS2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="W2:X2"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="AC2:AD2"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="N2:O2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>